<commit_message>
emilia checked Daily_Money_amount EOD_report Closing_The_Register get_inventory_report return_inventory add_new_inventory and added side notes.
</commit_message>
<xml_diff>
--- a/final project/EOD.xlsx
+++ b/final project/EOD.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="4">
   <si>
     <t>date</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>27 Dec 2018</t>
+  </si>
+  <si>
+    <t>02 Jan 2019</t>
   </si>
 </sst>
 </file>
@@ -354,7 +357,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -752,6 +755,54 @@
         <v>350</v>
       </c>
     </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50">
+        <v>499.8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51">
+        <v>499.8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52">
+        <v>499.8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53">
+        <v>499.8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54">
+        <v>499.8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55">
+        <v>499.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
in find costumer- input the id in the menu
</commit_message>
<xml_diff>
--- a/final project/EOD.xlsx
+++ b/final project/EOD.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>date</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>06 Jan 2019</t>
+  </si>
+  <si>
+    <t>07 Jan 2019</t>
   </si>
 </sst>
 </file>
@@ -363,7 +366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -409,6 +412,14 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>